<commit_message>
Update on project proposal 1.4
</commit_message>
<xml_diff>
--- a/documentation/Other documents/Project Schedule.xlsx
+++ b/documentation/Other documents/Project Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manethwijetunga/Development/Group_Project-_1/documentation/Other documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95D0E3D-AAE9-0A4A-9797-5747CD1BECEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB1993B-EA99-CD45-9348-CD2DFEA783DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -190,30 +190,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="6"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue Medium"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="6"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue Medium"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue Medium"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="6"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue Medium"/>
-    </font>
-    <font>
       <sz val="6"/>
       <color indexed="20"/>
       <name val="Helvetica Neue Medium"/>
@@ -223,8 +199,24 @@
       <color theme="1"/>
       <name val="Helvetica Neue Medium"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue Medium"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue Medium"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="7"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue Medium"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,6 +319,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -381,7 +379,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -397,23 +395,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -436,58 +422,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,10 +464,58 @@
     <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1902,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="V41" sqref="V41"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1994,75 +2001,75 @@
       <c r="BB1" s="3"/>
     </row>
     <row r="2" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7" t="s">
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7" t="s">
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7" t="s">
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7" t="s">
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7" t="s">
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="AM2" s="7"/>
-      <c r="AN2" s="7"/>
-      <c r="AO2" s="7"/>
-      <c r="AP2" s="7" t="s">
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="7"/>
-      <c r="AR2" s="7"/>
-      <c r="AS2" s="7"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
@@ -2074,137 +2081,137 @@
       <c r="BB2" s="3"/>
     </row>
     <row r="3" spans="1:54" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Y3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="Z3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AA3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AB3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AC3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AD3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AE3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AF3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AG3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AH3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AI3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AJ3" s="6" t="s">
+      <c r="AJ3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AK3" s="6" t="s">
+      <c r="AK3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AL3" s="6" t="s">
+      <c r="AL3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AM3" s="6" t="s">
+      <c r="AM3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AN3" s="6" t="s">
+      <c r="AN3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AO3" s="6" t="s">
+      <c r="AO3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AP3" s="6" t="s">
+      <c r="AP3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AQ3" s="6" t="s">
+      <c r="AQ3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AR3" s="6" t="s">
+      <c r="AR3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AS3" s="6" t="s">
+      <c r="AS3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="AT3" s="2"/>
@@ -2218,51 +2225,51 @@
       <c r="BB3" s="3"/>
     </row>
     <row r="4" spans="1:54" ht="8.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
-      <c r="AP4" s="9"/>
-      <c r="AQ4" s="9"/>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="9"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="6"/>
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
       <c r="AV4" s="2"/>
@@ -2274,53 +2281,53 @@
       <c r="BB4" s="3"/>
     </row>
     <row r="5" spans="1:54" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-      <c r="AS5" s="9"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AR5" s="6"/>
+      <c r="AS5" s="6"/>
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
       <c r="AV5" s="2"/>
@@ -2332,53 +2339,53 @@
       <c r="BB5" s="3"/>
     </row>
     <row r="6" spans="1:54" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15"/>
-      <c r="AO6" s="15"/>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="11"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="11"/>
+      <c r="AP6" s="11"/>
+      <c r="AQ6" s="11"/>
+      <c r="AR6" s="11"/>
+      <c r="AS6" s="11"/>
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
       <c r="AV6" s="2"/>
@@ -2390,53 +2397,53 @@
       <c r="BB6" s="3"/>
     </row>
     <row r="7" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="13"/>
-      <c r="AJ7" s="13"/>
-      <c r="AK7" s="13"/>
-      <c r="AL7" s="13"/>
-      <c r="AM7" s="13"/>
-      <c r="AN7" s="13"/>
-      <c r="AO7" s="13"/>
-      <c r="AP7" s="13"/>
-      <c r="AQ7" s="13"/>
-      <c r="AR7" s="13"/>
-      <c r="AS7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
       <c r="AV7" s="2"/>
@@ -2448,53 +2455,53 @@
       <c r="BB7" s="3"/>
     </row>
     <row r="8" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="15"/>
-      <c r="AC8" s="15"/>
-      <c r="AD8" s="15"/>
-      <c r="AE8" s="15"/>
-      <c r="AF8" s="15"/>
-      <c r="AG8" s="15"/>
-      <c r="AH8" s="15"/>
-      <c r="AI8" s="15"/>
-      <c r="AJ8" s="15"/>
-      <c r="AK8" s="15"/>
-      <c r="AL8" s="15"/>
-      <c r="AM8" s="15"/>
-      <c r="AN8" s="15"/>
-      <c r="AO8" s="15"/>
-      <c r="AP8" s="15"/>
-      <c r="AQ8" s="15"/>
-      <c r="AR8" s="15"/>
-      <c r="AS8" s="15"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="11"/>
+      <c r="AM8" s="11"/>
+      <c r="AN8" s="11"/>
+      <c r="AO8" s="11"/>
+      <c r="AP8" s="11"/>
+      <c r="AQ8" s="11"/>
+      <c r="AR8" s="11"/>
+      <c r="AS8" s="11"/>
       <c r="AT8" s="2"/>
       <c r="AU8" s="2"/>
       <c r="AV8" s="2"/>
@@ -2506,53 +2513,53 @@
       <c r="BB8" s="3"/>
     </row>
     <row r="9" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="13"/>
-      <c r="AI9" s="13"/>
-      <c r="AJ9" s="13"/>
-      <c r="AK9" s="13"/>
-      <c r="AL9" s="13"/>
-      <c r="AM9" s="13"/>
-      <c r="AN9" s="13"/>
-      <c r="AO9" s="13"/>
-      <c r="AP9" s="13"/>
-      <c r="AQ9" s="13"/>
-      <c r="AR9" s="13"/>
-      <c r="AS9" s="13"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9"/>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
       <c r="AV9" s="2"/>
@@ -2564,53 +2571,53 @@
       <c r="BB9" s="3"/>
     </row>
     <row r="10" spans="1:54" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="15"/>
-      <c r="AH10" s="15"/>
-      <c r="AI10" s="15"/>
-      <c r="AJ10" s="15"/>
-      <c r="AK10" s="15"/>
-      <c r="AL10" s="15"/>
-      <c r="AM10" s="15"/>
-      <c r="AN10" s="15"/>
-      <c r="AO10" s="15"/>
-      <c r="AP10" s="15"/>
-      <c r="AQ10" s="15"/>
-      <c r="AR10" s="15"/>
-      <c r="AS10" s="15"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="11"/>
+      <c r="AM10" s="11"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="11"/>
+      <c r="AP10" s="11"/>
+      <c r="AQ10" s="11"/>
+      <c r="AR10" s="11"/>
+      <c r="AS10" s="11"/>
       <c r="AT10" s="2"/>
       <c r="AU10" s="2"/>
       <c r="AV10" s="2"/>
@@ -2622,53 +2629,53 @@
       <c r="BB10" s="3"/>
     </row>
     <row r="11" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13"/>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="13"/>
-      <c r="AD11" s="13"/>
-      <c r="AE11" s="13"/>
-      <c r="AF11" s="13"/>
-      <c r="AG11" s="13"/>
-      <c r="AH11" s="13"/>
-      <c r="AI11" s="13"/>
-      <c r="AJ11" s="13"/>
-      <c r="AK11" s="13"/>
-      <c r="AL11" s="13"/>
-      <c r="AM11" s="13"/>
-      <c r="AN11" s="13"/>
-      <c r="AO11" s="13"/>
-      <c r="AP11" s="13"/>
-      <c r="AQ11" s="13"/>
-      <c r="AR11" s="13"/>
-      <c r="AS11" s="13"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
       <c r="AT11" s="2"/>
       <c r="AU11" s="2"/>
       <c r="AV11" s="2"/>
@@ -2680,53 +2687,53 @@
       <c r="BB11" s="3"/>
     </row>
     <row r="12" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13"/>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="13"/>
-      <c r="AD12" s="13"/>
-      <c r="AE12" s="13"/>
-      <c r="AF12" s="13"/>
-      <c r="AG12" s="13"/>
-      <c r="AH12" s="13"/>
-      <c r="AI12" s="13"/>
-      <c r="AJ12" s="13"/>
-      <c r="AK12" s="13"/>
-      <c r="AL12" s="13"/>
-      <c r="AM12" s="13"/>
-      <c r="AN12" s="13"/>
-      <c r="AO12" s="13"/>
-      <c r="AP12" s="13"/>
-      <c r="AQ12" s="13"/>
-      <c r="AR12" s="13"/>
-      <c r="AS12" s="13"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="9"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9"/>
       <c r="AT12" s="2"/>
       <c r="AU12" s="2"/>
       <c r="AV12" s="2"/>
@@ -2738,53 +2745,53 @@
       <c r="BB12" s="3"/>
     </row>
     <row r="13" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="13"/>
-      <c r="AB13" s="13"/>
-      <c r="AC13" s="13"/>
-      <c r="AD13" s="13"/>
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13"/>
-      <c r="AH13" s="13"/>
-      <c r="AI13" s="13"/>
-      <c r="AJ13" s="13"/>
-      <c r="AK13" s="13"/>
-      <c r="AL13" s="13"/>
-      <c r="AM13" s="13"/>
-      <c r="AN13" s="13"/>
-      <c r="AO13" s="13"/>
-      <c r="AP13" s="13"/>
-      <c r="AQ13" s="13"/>
-      <c r="AR13" s="13"/>
-      <c r="AS13" s="13"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
+      <c r="AM13" s="9"/>
+      <c r="AN13" s="9"/>
+      <c r="AO13" s="9"/>
+      <c r="AP13" s="9"/>
+      <c r="AQ13" s="9"/>
+      <c r="AR13" s="9"/>
+      <c r="AS13" s="9"/>
       <c r="AT13" s="2"/>
       <c r="AU13" s="2"/>
       <c r="AV13" s="2"/>
@@ -2796,53 +2803,53 @@
       <c r="BB13" s="3"/>
     </row>
     <row r="14" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="13"/>
-      <c r="AD14" s="13"/>
-      <c r="AE14" s="13"/>
-      <c r="AF14" s="13"/>
-      <c r="AG14" s="13"/>
-      <c r="AH14" s="13"/>
-      <c r="AI14" s="13"/>
-      <c r="AJ14" s="13"/>
-      <c r="AK14" s="13"/>
-      <c r="AL14" s="13"/>
-      <c r="AM14" s="13"/>
-      <c r="AN14" s="13"/>
-      <c r="AO14" s="13"/>
-      <c r="AP14" s="13"/>
-      <c r="AQ14" s="13"/>
-      <c r="AR14" s="13"/>
-      <c r="AS14" s="13"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+      <c r="AJ14" s="9"/>
+      <c r="AK14" s="9"/>
+      <c r="AL14" s="9"/>
+      <c r="AM14" s="9"/>
+      <c r="AN14" s="9"/>
+      <c r="AO14" s="9"/>
+      <c r="AP14" s="9"/>
+      <c r="AQ14" s="9"/>
+      <c r="AR14" s="9"/>
+      <c r="AS14" s="9"/>
       <c r="AT14" s="2"/>
       <c r="AU14" s="2"/>
       <c r="AV14" s="2"/>
@@ -2854,53 +2861,53 @@
       <c r="BB14" s="3"/>
     </row>
     <row r="15" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="15"/>
-      <c r="AD15" s="15"/>
-      <c r="AE15" s="15"/>
-      <c r="AF15" s="15"/>
-      <c r="AG15" s="15"/>
-      <c r="AH15" s="15"/>
-      <c r="AI15" s="15"/>
-      <c r="AJ15" s="15"/>
-      <c r="AK15" s="15"/>
-      <c r="AL15" s="15"/>
-      <c r="AM15" s="15"/>
-      <c r="AN15" s="15"/>
-      <c r="AO15" s="15"/>
-      <c r="AP15" s="15"/>
-      <c r="AQ15" s="15"/>
-      <c r="AR15" s="15"/>
-      <c r="AS15" s="15"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="11"/>
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="11"/>
+      <c r="AL15" s="11"/>
+      <c r="AM15" s="11"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
+      <c r="AQ15" s="11"/>
+      <c r="AR15" s="11"/>
+      <c r="AS15" s="11"/>
       <c r="AT15" s="2"/>
       <c r="AU15" s="2"/>
       <c r="AV15" s="2"/>
@@ -2912,53 +2919,53 @@
       <c r="BB15" s="3"/>
     </row>
     <row r="16" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13"/>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="13"/>
-      <c r="AB16" s="13"/>
-      <c r="AC16" s="13"/>
-      <c r="AD16" s="13"/>
-      <c r="AE16" s="13"/>
-      <c r="AF16" s="13"/>
-      <c r="AG16" s="13"/>
-      <c r="AH16" s="13"/>
-      <c r="AI16" s="13"/>
-      <c r="AJ16" s="13"/>
-      <c r="AK16" s="13"/>
-      <c r="AL16" s="13"/>
-      <c r="AM16" s="13"/>
-      <c r="AN16" s="13"/>
-      <c r="AO16" s="13"/>
-      <c r="AP16" s="13"/>
-      <c r="AQ16" s="13"/>
-      <c r="AR16" s="13"/>
-      <c r="AS16" s="13"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="9"/>
+      <c r="AL16" s="9"/>
+      <c r="AM16" s="9"/>
+      <c r="AN16" s="9"/>
+      <c r="AO16" s="9"/>
+      <c r="AP16" s="9"/>
+      <c r="AQ16" s="9"/>
+      <c r="AR16" s="9"/>
+      <c r="AS16" s="9"/>
       <c r="AT16" s="2"/>
       <c r="AU16" s="2"/>
       <c r="AV16" s="2"/>
@@ -2970,53 +2977,53 @@
       <c r="BB16" s="3"/>
     </row>
     <row r="17" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="13"/>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="13"/>
-      <c r="AJ17" s="13"/>
-      <c r="AK17" s="13"/>
-      <c r="AL17" s="13"/>
-      <c r="AM17" s="13"/>
-      <c r="AN17" s="13"/>
-      <c r="AO17" s="13"/>
-      <c r="AP17" s="13"/>
-      <c r="AQ17" s="13"/>
-      <c r="AR17" s="13"/>
-      <c r="AS17" s="13"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="9"/>
+      <c r="AL17" s="9"/>
+      <c r="AM17" s="9"/>
+      <c r="AN17" s="9"/>
+      <c r="AO17" s="9"/>
+      <c r="AP17" s="9"/>
+      <c r="AQ17" s="9"/>
+      <c r="AR17" s="9"/>
+      <c r="AS17" s="9"/>
       <c r="AT17" s="2"/>
       <c r="AU17" s="2"/>
       <c r="AV17" s="2"/>
@@ -3028,53 +3035,53 @@
       <c r="BB17" s="3"/>
     </row>
     <row r="18" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="15"/>
-      <c r="AC18" s="15"/>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="15"/>
-      <c r="AF18" s="15"/>
-      <c r="AG18" s="15"/>
-      <c r="AH18" s="15"/>
-      <c r="AI18" s="15"/>
-      <c r="AJ18" s="15"/>
-      <c r="AK18" s="15"/>
-      <c r="AL18" s="15"/>
-      <c r="AM18" s="15"/>
-      <c r="AN18" s="15"/>
-      <c r="AO18" s="15"/>
-      <c r="AP18" s="15"/>
-      <c r="AQ18" s="15"/>
-      <c r="AR18" s="15"/>
-      <c r="AS18" s="15"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="11"/>
+      <c r="AK18" s="11"/>
+      <c r="AL18" s="11"/>
+      <c r="AM18" s="11"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="11"/>
+      <c r="AP18" s="11"/>
+      <c r="AQ18" s="11"/>
+      <c r="AR18" s="11"/>
+      <c r="AS18" s="11"/>
       <c r="AT18" s="2"/>
       <c r="AU18" s="2"/>
       <c r="AV18" s="2"/>
@@ -3086,53 +3093,53 @@
       <c r="BB18" s="3"/>
     </row>
     <row r="19" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="27"/>
-      <c r="Z19" s="27"/>
-      <c r="AA19" s="27"/>
-      <c r="AB19" s="27"/>
-      <c r="AC19" s="27"/>
-      <c r="AD19" s="27"/>
-      <c r="AE19" s="13"/>
-      <c r="AF19" s="13"/>
-      <c r="AG19" s="13"/>
-      <c r="AH19" s="13"/>
-      <c r="AI19" s="13"/>
-      <c r="AJ19" s="13"/>
-      <c r="AK19" s="13"/>
-      <c r="AL19" s="13"/>
-      <c r="AM19" s="13"/>
-      <c r="AN19" s="13"/>
-      <c r="AO19" s="13"/>
-      <c r="AP19" s="13"/>
-      <c r="AQ19" s="13"/>
-      <c r="AR19" s="13"/>
-      <c r="AS19" s="13"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="18"/>
+      <c r="W19" s="18"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="18"/>
+      <c r="AA19" s="18"/>
+      <c r="AB19" s="18"/>
+      <c r="AC19" s="18"/>
+      <c r="AD19" s="18"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
+      <c r="AL19" s="9"/>
+      <c r="AM19" s="9"/>
+      <c r="AN19" s="9"/>
+      <c r="AO19" s="9"/>
+      <c r="AP19" s="9"/>
+      <c r="AQ19" s="9"/>
+      <c r="AR19" s="9"/>
+      <c r="AS19" s="9"/>
       <c r="AT19" s="2"/>
       <c r="AU19" s="2"/>
       <c r="AV19" s="2"/>
@@ -3144,53 +3151,53 @@
       <c r="BB19" s="3"/>
     </row>
     <row r="20" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
-      <c r="Y20" s="13"/>
-      <c r="Z20" s="13"/>
-      <c r="AA20" s="13"/>
-      <c r="AB20" s="13"/>
-      <c r="AC20" s="13"/>
-      <c r="AD20" s="13"/>
-      <c r="AE20" s="13"/>
-      <c r="AF20" s="13"/>
-      <c r="AG20" s="13"/>
-      <c r="AH20" s="13"/>
-      <c r="AI20" s="13"/>
-      <c r="AJ20" s="13"/>
-      <c r="AK20" s="13"/>
-      <c r="AL20" s="13"/>
-      <c r="AM20" s="13"/>
-      <c r="AN20" s="13"/>
-      <c r="AO20" s="13"/>
-      <c r="AP20" s="13"/>
-      <c r="AQ20" s="13"/>
-      <c r="AR20" s="13"/>
-      <c r="AS20" s="13"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
+      <c r="AK20" s="9"/>
+      <c r="AL20" s="9"/>
+      <c r="AM20" s="9"/>
+      <c r="AN20" s="9"/>
+      <c r="AO20" s="9"/>
+      <c r="AP20" s="9"/>
+      <c r="AQ20" s="9"/>
+      <c r="AR20" s="9"/>
+      <c r="AS20" s="9"/>
       <c r="AT20" s="2"/>
       <c r="AU20" s="2"/>
       <c r="AV20" s="2"/>
@@ -3202,53 +3209,53 @@
       <c r="BB20" s="3"/>
     </row>
     <row r="21" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="22"/>
-      <c r="U21" s="22"/>
-      <c r="V21" s="22"/>
-      <c r="W21" s="22"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="13"/>
-      <c r="AB21" s="13"/>
-      <c r="AC21" s="13"/>
-      <c r="AD21" s="13"/>
-      <c r="AE21" s="13"/>
-      <c r="AF21" s="13"/>
-      <c r="AG21" s="13"/>
-      <c r="AH21" s="13"/>
-      <c r="AI21" s="13"/>
-      <c r="AJ21" s="13"/>
-      <c r="AK21" s="13"/>
-      <c r="AL21" s="13"/>
-      <c r="AM21" s="13"/>
-      <c r="AN21" s="13"/>
-      <c r="AO21" s="13"/>
-      <c r="AP21" s="13"/>
-      <c r="AQ21" s="13"/>
-      <c r="AR21" s="13"/>
-      <c r="AS21" s="13"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="9"/>
+      <c r="AL21" s="9"/>
+      <c r="AM21" s="9"/>
+      <c r="AN21" s="9"/>
+      <c r="AO21" s="9"/>
+      <c r="AP21" s="9"/>
+      <c r="AQ21" s="9"/>
+      <c r="AR21" s="9"/>
+      <c r="AS21" s="9"/>
       <c r="AT21" s="2"/>
       <c r="AU21" s="2"/>
       <c r="AV21" s="2"/>
@@ -3260,53 +3267,53 @@
       <c r="BB21" s="3"/>
     </row>
     <row r="22" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="25"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="30"/>
-      <c r="Y22" s="30"/>
-      <c r="Z22" s="30"/>
-      <c r="AA22" s="30"/>
-      <c r="AB22" s="30"/>
-      <c r="AC22" s="15"/>
-      <c r="AD22" s="15"/>
-      <c r="AE22" s="15"/>
-      <c r="AF22" s="15"/>
-      <c r="AG22" s="15"/>
-      <c r="AH22" s="15"/>
-      <c r="AI22" s="15"/>
-      <c r="AJ22" s="15"/>
-      <c r="AK22" s="15"/>
-      <c r="AL22" s="15"/>
-      <c r="AM22" s="15"/>
-      <c r="AN22" s="15"/>
-      <c r="AO22" s="15"/>
-      <c r="AP22" s="15"/>
-      <c r="AQ22" s="15"/>
-      <c r="AR22" s="15"/>
-      <c r="AS22" s="15"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="20"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+      <c r="AE22" s="11"/>
+      <c r="AF22" s="11"/>
+      <c r="AG22" s="11"/>
+      <c r="AH22" s="11"/>
+      <c r="AI22" s="11"/>
+      <c r="AJ22" s="11"/>
+      <c r="AK22" s="11"/>
+      <c r="AL22" s="11"/>
+      <c r="AM22" s="11"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="11"/>
+      <c r="AP22" s="11"/>
+      <c r="AQ22" s="11"/>
+      <c r="AR22" s="11"/>
+      <c r="AS22" s="11"/>
       <c r="AT22" s="2"/>
       <c r="AU22" s="2"/>
       <c r="AV22" s="2"/>
@@ -3318,53 +3325,53 @@
       <c r="BB22" s="3"/>
     </row>
     <row r="23" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
-      <c r="AA23" s="30"/>
-      <c r="AB23" s="30"/>
-      <c r="AC23" s="30"/>
-      <c r="AD23" s="16"/>
-      <c r="AE23" s="13"/>
-      <c r="AF23" s="13"/>
-      <c r="AG23" s="13"/>
-      <c r="AH23" s="13"/>
-      <c r="AI23" s="13"/>
-      <c r="AJ23" s="13"/>
-      <c r="AK23" s="13"/>
-      <c r="AL23" s="13"/>
-      <c r="AM23" s="13"/>
-      <c r="AN23" s="13"/>
-      <c r="AO23" s="13"/>
-      <c r="AP23" s="13"/>
-      <c r="AQ23" s="13"/>
-      <c r="AR23" s="13"/>
-      <c r="AS23" s="13"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="20"/>
+      <c r="AD23" s="12"/>
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="9"/>
+      <c r="AJ23" s="9"/>
+      <c r="AK23" s="9"/>
+      <c r="AL23" s="9"/>
+      <c r="AM23" s="9"/>
+      <c r="AN23" s="9"/>
+      <c r="AO23" s="9"/>
+      <c r="AP23" s="9"/>
+      <c r="AQ23" s="9"/>
+      <c r="AR23" s="9"/>
+      <c r="AS23" s="9"/>
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
       <c r="AV23" s="2"/>
@@ -3376,53 +3383,53 @@
       <c r="BB23" s="3"/>
     </row>
     <row r="24" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
-      <c r="AA24" s="15"/>
-      <c r="AB24" s="15"/>
-      <c r="AC24" s="30"/>
-      <c r="AD24" s="30"/>
-      <c r="AE24" s="16"/>
-      <c r="AF24" s="16"/>
-      <c r="AG24" s="16"/>
-      <c r="AH24" s="15"/>
-      <c r="AI24" s="15"/>
-      <c r="AJ24" s="15"/>
-      <c r="AK24" s="15"/>
-      <c r="AL24" s="15"/>
-      <c r="AM24" s="15"/>
-      <c r="AN24" s="15"/>
-      <c r="AO24" s="15"/>
-      <c r="AP24" s="15"/>
-      <c r="AQ24" s="15"/>
-      <c r="AR24" s="15"/>
-      <c r="AS24" s="15"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="20"/>
+      <c r="AD24" s="31"/>
+      <c r="AE24" s="12"/>
+      <c r="AF24" s="12"/>
+      <c r="AG24" s="12"/>
+      <c r="AH24" s="11"/>
+      <c r="AI24" s="11"/>
+      <c r="AJ24" s="11"/>
+      <c r="AK24" s="11"/>
+      <c r="AL24" s="11"/>
+      <c r="AM24" s="11"/>
+      <c r="AN24" s="11"/>
+      <c r="AO24" s="11"/>
+      <c r="AP24" s="11"/>
+      <c r="AQ24" s="11"/>
+      <c r="AR24" s="11"/>
+      <c r="AS24" s="11"/>
       <c r="AT24" s="2"/>
       <c r="AU24" s="2"/>
       <c r="AV24" s="2"/>
@@ -3434,53 +3441,53 @@
       <c r="BB24" s="3"/>
     </row>
     <row r="25" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="13"/>
-      <c r="X25" s="13"/>
-      <c r="Y25" s="13"/>
-      <c r="Z25" s="13"/>
-      <c r="AA25" s="13"/>
-      <c r="AB25" s="13"/>
-      <c r="AC25" s="13"/>
-      <c r="AD25" s="36"/>
-      <c r="AE25" s="36"/>
-      <c r="AF25" s="36"/>
-      <c r="AG25" s="36"/>
-      <c r="AH25" s="36"/>
-      <c r="AI25" s="36"/>
-      <c r="AJ25" s="36"/>
-      <c r="AK25" s="36"/>
-      <c r="AL25" s="16"/>
-      <c r="AM25" s="16"/>
-      <c r="AN25" s="16"/>
-      <c r="AO25" s="16"/>
-      <c r="AP25" s="13"/>
-      <c r="AQ25" s="13"/>
-      <c r="AR25" s="13"/>
-      <c r="AS25" s="13"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="23"/>
+      <c r="AE25" s="23"/>
+      <c r="AF25" s="23"/>
+      <c r="AG25" s="23"/>
+      <c r="AH25" s="23"/>
+      <c r="AI25" s="23"/>
+      <c r="AJ25" s="23"/>
+      <c r="AK25" s="23"/>
+      <c r="AL25" s="12"/>
+      <c r="AM25" s="12"/>
+      <c r="AN25" s="12"/>
+      <c r="AO25" s="12"/>
+      <c r="AP25" s="9"/>
+      <c r="AQ25" s="9"/>
+      <c r="AR25" s="9"/>
+      <c r="AS25" s="9"/>
       <c r="AT25" s="2"/>
       <c r="AU25" s="2"/>
       <c r="AV25" s="2"/>
@@ -3492,53 +3499,53 @@
       <c r="BB25" s="3"/>
     </row>
     <row r="26" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
-      <c r="AA26" s="15"/>
-      <c r="AB26" s="15"/>
-      <c r="AC26" s="15"/>
-      <c r="AD26" s="37"/>
-      <c r="AE26" s="37"/>
-      <c r="AF26" s="37"/>
-      <c r="AG26" s="15"/>
-      <c r="AH26" s="16"/>
-      <c r="AI26" s="16"/>
-      <c r="AJ26" s="16"/>
-      <c r="AK26" s="16"/>
-      <c r="AL26" s="16"/>
-      <c r="AM26" s="16"/>
-      <c r="AN26" s="16"/>
-      <c r="AO26" s="16"/>
-      <c r="AP26" s="15"/>
-      <c r="AQ26" s="15"/>
-      <c r="AR26" s="15"/>
-      <c r="AS26" s="15"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="24"/>
+      <c r="AE26" s="24"/>
+      <c r="AF26" s="24"/>
+      <c r="AG26" s="11"/>
+      <c r="AH26" s="12"/>
+      <c r="AI26" s="12"/>
+      <c r="AJ26" s="12"/>
+      <c r="AK26" s="12"/>
+      <c r="AL26" s="12"/>
+      <c r="AM26" s="12"/>
+      <c r="AN26" s="12"/>
+      <c r="AO26" s="12"/>
+      <c r="AP26" s="11"/>
+      <c r="AQ26" s="11"/>
+      <c r="AR26" s="11"/>
+      <c r="AS26" s="11"/>
       <c r="AT26" s="2"/>
       <c r="AU26" s="2"/>
       <c r="AV26" s="2"/>
@@ -3550,53 +3557,53 @@
       <c r="BB26" s="3"/>
     </row>
     <row r="27" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-      <c r="AA27" s="13"/>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
-      <c r="AD27" s="13"/>
-      <c r="AE27" s="13"/>
-      <c r="AF27" s="37"/>
-      <c r="AG27" s="37"/>
-      <c r="AH27" s="37"/>
-      <c r="AI27" s="13"/>
-      <c r="AJ27" s="13"/>
-      <c r="AK27" s="13"/>
-      <c r="AL27" s="13"/>
-      <c r="AM27" s="16"/>
-      <c r="AN27" s="16"/>
-      <c r="AO27" s="16"/>
-      <c r="AP27" s="16"/>
-      <c r="AQ27" s="16"/>
-      <c r="AR27" s="16"/>
-      <c r="AS27" s="16"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="9"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="24"/>
+      <c r="AG27" s="24"/>
+      <c r="AH27" s="24"/>
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="9"/>
+      <c r="AK27" s="9"/>
+      <c r="AL27" s="9"/>
+      <c r="AM27" s="12"/>
+      <c r="AN27" s="12"/>
+      <c r="AO27" s="12"/>
+      <c r="AP27" s="12"/>
+      <c r="AQ27" s="12"/>
+      <c r="AR27" s="12"/>
+      <c r="AS27" s="12"/>
       <c r="AT27" s="2"/>
       <c r="AU27" s="2"/>
       <c r="AV27" s="2"/>
@@ -3608,53 +3615,53 @@
       <c r="BB27" s="3"/>
     </row>
     <row r="28" spans="1:54" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="15"/>
-      <c r="W28" s="15"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="15"/>
-      <c r="Z28" s="15"/>
-      <c r="AA28" s="15"/>
-      <c r="AB28" s="15"/>
-      <c r="AC28" s="15"/>
-      <c r="AD28" s="15"/>
-      <c r="AE28" s="15"/>
-      <c r="AF28" s="15"/>
-      <c r="AG28" s="16"/>
-      <c r="AH28" s="37"/>
-      <c r="AI28" s="37"/>
-      <c r="AJ28" s="15"/>
-      <c r="AK28" s="15"/>
-      <c r="AL28" s="15"/>
-      <c r="AM28" s="16"/>
-      <c r="AN28" s="16"/>
-      <c r="AO28" s="16"/>
-      <c r="AP28" s="16"/>
-      <c r="AQ28" s="16"/>
-      <c r="AR28" s="16"/>
-      <c r="AS28" s="16"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="11"/>
+      <c r="AE28" s="11"/>
+      <c r="AF28" s="11"/>
+      <c r="AG28" s="12"/>
+      <c r="AH28" s="24"/>
+      <c r="AI28" s="24"/>
+      <c r="AJ28" s="11"/>
+      <c r="AK28" s="11"/>
+      <c r="AL28" s="11"/>
+      <c r="AM28" s="12"/>
+      <c r="AN28" s="12"/>
+      <c r="AO28" s="12"/>
+      <c r="AP28" s="12"/>
+      <c r="AQ28" s="12"/>
+      <c r="AR28" s="12"/>
+      <c r="AS28" s="12"/>
       <c r="AT28" s="2"/>
       <c r="AU28" s="2"/>
       <c r="AV28" s="2"/>
@@ -3666,53 +3673,53 @@
       <c r="BB28" s="3"/>
     </row>
     <row r="29" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17"/>
-      <c r="U29" s="17"/>
-      <c r="V29" s="17"/>
-      <c r="W29" s="17"/>
-      <c r="X29" s="17"/>
-      <c r="Y29" s="17"/>
-      <c r="Z29" s="17"/>
-      <c r="AA29" s="17"/>
-      <c r="AB29" s="17"/>
-      <c r="AC29" s="17"/>
-      <c r="AD29" s="17"/>
-      <c r="AE29" s="17"/>
-      <c r="AF29" s="17"/>
-      <c r="AG29" s="17"/>
-      <c r="AH29" s="38"/>
-      <c r="AI29" s="39"/>
-      <c r="AJ29" s="39"/>
-      <c r="AK29" s="39"/>
-      <c r="AL29" s="17"/>
-      <c r="AM29" s="38"/>
-      <c r="AN29" s="38"/>
-      <c r="AO29" s="38"/>
-      <c r="AP29" s="38"/>
-      <c r="AQ29" s="38"/>
-      <c r="AR29" s="38"/>
-      <c r="AS29" s="38"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+      <c r="W29" s="13"/>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
+      <c r="Z29" s="13"/>
+      <c r="AA29" s="13"/>
+      <c r="AB29" s="13"/>
+      <c r="AC29" s="13"/>
+      <c r="AD29" s="13"/>
+      <c r="AE29" s="13"/>
+      <c r="AF29" s="13"/>
+      <c r="AG29" s="13"/>
+      <c r="AH29" s="25"/>
+      <c r="AI29" s="26"/>
+      <c r="AJ29" s="26"/>
+      <c r="AK29" s="26"/>
+      <c r="AL29" s="13"/>
+      <c r="AM29" s="25"/>
+      <c r="AN29" s="25"/>
+      <c r="AO29" s="25"/>
+      <c r="AP29" s="25"/>
+      <c r="AQ29" s="25"/>
+      <c r="AR29" s="25"/>
+      <c r="AS29" s="25"/>
       <c r="AT29" s="2"/>
       <c r="AU29" s="2"/>
       <c r="AV29" s="2"/>
@@ -3724,53 +3731,53 @@
       <c r="BB29" s="3"/>
     </row>
     <row r="30" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="17"/>
-      <c r="V30" s="17"/>
-      <c r="W30" s="17"/>
-      <c r="X30" s="17"/>
-      <c r="Y30" s="17"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="17"/>
-      <c r="AB30" s="17"/>
-      <c r="AC30" s="17"/>
-      <c r="AD30" s="17"/>
-      <c r="AE30" s="17"/>
-      <c r="AF30" s="17"/>
-      <c r="AG30" s="17"/>
-      <c r="AH30" s="17"/>
-      <c r="AI30" s="17"/>
-      <c r="AJ30" s="17"/>
-      <c r="AK30" s="17"/>
-      <c r="AL30" s="40"/>
-      <c r="AM30" s="40"/>
-      <c r="AN30" s="40"/>
-      <c r="AO30" s="40"/>
-      <c r="AP30" s="40"/>
-      <c r="AQ30" s="40"/>
-      <c r="AR30" s="40"/>
-      <c r="AS30" s="40"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="13"/>
+      <c r="AA30" s="13"/>
+      <c r="AB30" s="13"/>
+      <c r="AC30" s="13"/>
+      <c r="AD30" s="13"/>
+      <c r="AE30" s="13"/>
+      <c r="AF30" s="13"/>
+      <c r="AG30" s="13"/>
+      <c r="AH30" s="13"/>
+      <c r="AI30" s="13"/>
+      <c r="AJ30" s="13"/>
+      <c r="AK30" s="13"/>
+      <c r="AL30" s="27"/>
+      <c r="AM30" s="27"/>
+      <c r="AN30" s="27"/>
+      <c r="AO30" s="27"/>
+      <c r="AP30" s="27"/>
+      <c r="AQ30" s="27"/>
+      <c r="AR30" s="27"/>
+      <c r="AS30" s="27"/>
       <c r="AT30" s="2"/>
       <c r="AU30" s="2"/>
       <c r="AV30" s="2"/>
@@ -3782,53 +3789,53 @@
       <c r="BB30" s="3"/>
     </row>
     <row r="31" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="17"/>
-      <c r="U31" s="17"/>
-      <c r="V31" s="17"/>
-      <c r="W31" s="17"/>
-      <c r="X31" s="17"/>
-      <c r="Y31" s="17"/>
-      <c r="Z31" s="17"/>
-      <c r="AA31" s="17"/>
-      <c r="AB31" s="17"/>
-      <c r="AC31" s="17"/>
-      <c r="AD31" s="17"/>
-      <c r="AE31" s="17"/>
-      <c r="AF31" s="17"/>
-      <c r="AG31" s="17"/>
-      <c r="AH31" s="17"/>
-      <c r="AI31" s="17"/>
-      <c r="AJ31" s="17"/>
-      <c r="AK31" s="17"/>
-      <c r="AL31" s="41"/>
-      <c r="AM31" s="42"/>
-      <c r="AN31" s="42"/>
-      <c r="AO31" s="17"/>
-      <c r="AP31" s="17"/>
-      <c r="AQ31" s="17"/>
-      <c r="AR31" s="17"/>
-      <c r="AS31" s="17"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="13"/>
+      <c r="AB31" s="13"/>
+      <c r="AC31" s="13"/>
+      <c r="AD31" s="13"/>
+      <c r="AE31" s="13"/>
+      <c r="AF31" s="13"/>
+      <c r="AG31" s="13"/>
+      <c r="AH31" s="13"/>
+      <c r="AI31" s="13"/>
+      <c r="AJ31" s="13"/>
+      <c r="AK31" s="13"/>
+      <c r="AL31" s="28"/>
+      <c r="AM31" s="29"/>
+      <c r="AN31" s="29"/>
+      <c r="AO31" s="13"/>
+      <c r="AP31" s="13"/>
+      <c r="AQ31" s="13"/>
+      <c r="AR31" s="13"/>
+      <c r="AS31" s="13"/>
       <c r="AT31" s="2"/>
       <c r="AU31" s="2"/>
       <c r="AV31" s="2"/>
@@ -3840,53 +3847,53 @@
       <c r="BB31" s="3"/>
     </row>
     <row r="32" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
-      <c r="V32" s="17"/>
-      <c r="W32" s="17"/>
-      <c r="X32" s="17"/>
-      <c r="Y32" s="17"/>
-      <c r="Z32" s="17"/>
-      <c r="AA32" s="17"/>
-      <c r="AB32" s="17"/>
-      <c r="AC32" s="17"/>
-      <c r="AD32" s="17"/>
-      <c r="AE32" s="17"/>
-      <c r="AF32" s="17"/>
-      <c r="AG32" s="17"/>
-      <c r="AH32" s="17"/>
-      <c r="AI32" s="17"/>
-      <c r="AJ32" s="17"/>
-      <c r="AK32" s="17"/>
-      <c r="AL32" s="17"/>
-      <c r="AM32" s="17"/>
-      <c r="AN32" s="42"/>
-      <c r="AO32" s="42"/>
-      <c r="AP32" s="42"/>
-      <c r="AQ32" s="42"/>
-      <c r="AR32" s="42"/>
-      <c r="AS32" s="42"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+      <c r="AA32" s="13"/>
+      <c r="AB32" s="13"/>
+      <c r="AC32" s="13"/>
+      <c r="AD32" s="13"/>
+      <c r="AE32" s="13"/>
+      <c r="AF32" s="13"/>
+      <c r="AG32" s="13"/>
+      <c r="AH32" s="13"/>
+      <c r="AI32" s="13"/>
+      <c r="AJ32" s="13"/>
+      <c r="AK32" s="13"/>
+      <c r="AL32" s="13"/>
+      <c r="AM32" s="13"/>
+      <c r="AN32" s="29"/>
+      <c r="AO32" s="29"/>
+      <c r="AP32" s="29"/>
+      <c r="AQ32" s="29"/>
+      <c r="AR32" s="29"/>
+      <c r="AS32" s="29"/>
       <c r="AT32" s="2"/>
       <c r="AU32" s="2"/>
       <c r="AV32" s="2"/>
@@ -7651,18 +7658,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="Y2:AB2"/>
-    <mergeCell ref="AC2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="A4:D4"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="P2:T2"/>
     <mergeCell ref="U2:X2"/>
-    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="Y2:AB2"/>
+    <mergeCell ref="AC2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
   </mergeCells>
   <pageMargins left="0.375" right="0.375" top="0.76388900000000004" bottom="0.27777800000000002" header="0.25" footer="0.25"/>
   <pageSetup orientation="landscape"/>

</xml_diff>